<commit_message>
Introduce calculation to determine f-nought
</commit_message>
<xml_diff>
--- a/data/cant_solve_txt_4PL.xlsx
+++ b/data/cant_solve_txt_4PL.xlsx
@@ -16,13 +16,40 @@
     <definedName name="_B">Sheet1!$D$4</definedName>
     <definedName name="_C">Sheet1!$D$5</definedName>
     <definedName name="_D">Sheet1!$D$6</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$D$3:$D$6</definedName>
+    <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mip" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="0" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="0" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$7</definedName>
+    <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="0" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="0" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="0" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="0" hidden="1">2</definedName>
+    <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="0" hidden="1">3</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>X</t>
   </si>
@@ -49,6 +76,9 @@
   </si>
   <si>
     <t>diff</t>
+  </si>
+  <si>
+    <t>base freq:</t>
   </si>
 </sst>
 </file>
@@ -143,31 +173,37 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6511627906976702E-2</c:v>
+                  <c:v>1.9138755980861202E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16279069767441801</c:v>
+                  <c:v>0.105263157894736</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25581395348837199</c:v>
+                  <c:v>0.23923444976076499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38372093023255799</c:v>
+                  <c:v>0.36363636363636298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59302325581395299</c:v>
+                  <c:v>0.42105263157894701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70930232558139505</c:v>
+                  <c:v>0.46411483253588498</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.82558139534883701</c:v>
+                  <c:v>0.52631578947368396</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94186046511627897</c:v>
+                  <c:v>0.602870813397129</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1</c:v>
+                  <c:v>0.68899521531100405</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72727272727272696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.81339712918660201</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -179,34 +215,40 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>50.704000000000001</c:v>
+                  <c:v>50.685000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.673000000000002</c:v>
+                  <c:v>50.681999999999903</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.546999999999997</c:v>
+                  <c:v>50.673999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.361999999999902</c:v>
+                  <c:v>50.657999999999902</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.961999999999897</c:v>
+                  <c:v>50.622999999999898</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.436</c:v>
+                  <c:v>50.580999999999896</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.317</c:v>
+                  <c:v>50.538999999999902</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49.256</c:v>
+                  <c:v>50.461999999999897</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49.222999999999999</c:v>
+                  <c:v>50.34</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49.211999999999897</c:v>
+                  <c:v>50.09</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.835000000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.633000000000003</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -226,38 +268,53 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$19</c:f>
+              <c:f>Sheet1!$A$10:$A$24</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.6511627906976702E-2</c:v>
+                  <c:v>1.9138755980861202E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.16279069767441801</c:v>
+                  <c:v>0.105263157894736</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.25581395348837199</c:v>
+                  <c:v>0.23923444976076499</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38372093023255799</c:v>
+                  <c:v>0.36363636363636298</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.59302325581395299</c:v>
+                  <c:v>0.42105263157894701</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.70930232558139505</c:v>
+                  <c:v>0.46411483253588498</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.82558139534883701</c:v>
+                  <c:v>0.52631578947368396</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.94186046511627897</c:v>
+                  <c:v>0.602870813397129</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.68899521531100405</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.72727272727272696</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.81339712918660201</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>0.88038277511961704</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>0.93301435406698496</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -265,39 +322,54 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$C$19</c:f>
+              <c:f>Sheet1!$C$10:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="10"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>50.673220000000001</c:v>
+                  <c:v>50.654528760564574</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.671640058356296</c:v>
+                  <c:v>50.654528760537161</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.586727215774317</c:v>
+                  <c:v>50.654525648316636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.357576279510525</c:v>
+                  <c:v>50.653682928113923</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>49.917025894451392</c:v>
+                  <c:v>50.639919803518204</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.437775364875939</c:v>
+                  <c:v>50.615476442121121</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>49.315507514739672</c:v>
+                  <c:v>50.580543129138263</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>49.245698452572888</c:v>
+                  <c:v>50.491574295022247</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>49.204392461448776</c:v>
+                  <c:v>50.304616627082346</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>49.190178276201856</c:v>
+                  <c:v>50.019155844334179</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>49.88978625402887</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>49.643465936849829</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>49.509229532306399</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>49.435294422396581</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>49.371073513231082</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -312,11 +384,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="158180480"/>
-        <c:axId val="158145920"/>
+        <c:axId val="297686912"/>
+        <c:axId val="297688448"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="158180480"/>
+        <c:axId val="297686912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -326,12 +398,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158145920"/>
+        <c:crossAx val="297688448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="158145920"/>
+        <c:axId val="297688448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -342,7 +414,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158180480"/>
+        <c:crossAx val="297686912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -369,15 +441,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>204787</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>123825</xdr:rowOff>
+      <xdr:colOff>157162</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>509587</xdr:colOff>
-      <xdr:row>38</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>461962</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -398,16 +470,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>285750</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>456645</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>323295</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>180908</xdr:rowOff>
+      <xdr:rowOff>152333</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -424,7 +496,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3333750" y="219075"/>
+          <a:off x="5029200" y="190500"/>
           <a:ext cx="4438095" cy="533333"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -436,16 +508,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
       <xdr:row>4</xdr:row>
-      <xdr:rowOff>85240</xdr:rowOff>
+      <xdr:rowOff>56665</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>123170</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>9048</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>75545</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>170973</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -462,7 +534,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="3362325" y="847240"/>
+          <a:off x="5143500" y="818665"/>
           <a:ext cx="4076045" cy="2971808"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -762,20 +834,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H21"/>
+  <dimension ref="A3:H24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K30" sqref="K30"/>
+      <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="6" max="6" width="10.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>2</v>
       </c>
       <c r="D3">
-        <v>50.673220000000001</v>
+        <v>50.654528760564574</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -783,7 +858,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>3.24</v>
+        <v>6.8279031260186276</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -791,7 +866,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.39</v>
+        <v>0.70871416441597912</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -799,7 +874,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>49.12</v>
+        <v>49.248777592008274</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -807,8 +882,15 @@
         <v>6</v>
       </c>
       <c r="D7">
-        <f>SUM(D10:D19)</f>
-        <v>5.5036784198511648E-3</v>
+        <f>SUM(D10:D24)</f>
+        <v>1.7639332490389022E-2</v>
+      </c>
+      <c r="F7" t="s">
+        <v>9</v>
+      </c>
+      <c r="G7">
+        <f>_D+(_A-_D)/(1+POWER(_C/_C,_B))</f>
+        <v>49.951653176286428</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -830,176 +912,250 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>50.704000000000001</v>
+        <v>50.685000000000002</v>
       </c>
       <c r="C10">
-        <f>_D+(_A-_D)/(1+POWER(A10/_C,_B))</f>
-        <v>50.673220000000001</v>
+        <f>IF(ISBLANK(A10),0,_D+(_A-_D)/(1+POWER(A10/_C,_B)))</f>
+        <v>50.654528760564574</v>
       </c>
       <c r="D10">
         <f>POWER(C10-B10,2)</f>
-        <v>9.4740840000000182E-4</v>
+        <v>9.2849643273120006E-4</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>4.6511627906976702E-2</v>
+        <v>1.9138755980861202E-2</v>
       </c>
       <c r="B11">
-        <v>50.673000000000002</v>
+        <v>50.681999999999903</v>
       </c>
       <c r="C11">
-        <f>_D+(_A-_D)/(1+POWER(A11/_C,_B))</f>
-        <v>50.671640058356296</v>
+        <f>IF(ISBLANK(A11),0,_D+(_A-_D)/(1+POWER(A11/_C,_B)))</f>
+        <v>50.654528760537161</v>
       </c>
       <c r="D11">
         <f t="shared" ref="D11:D19" si="0">POWER(C11-B11,2)</f>
-        <v>1.8494412742858004E-6</v>
+        <v>7.5466899761928244E-4</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>0.16279069767441801</v>
+        <v>0.105263157894736</v>
       </c>
       <c r="B12">
-        <v>50.546999999999997</v>
+        <v>50.673999999999999</v>
       </c>
       <c r="C12">
-        <f>_D+(_A-_D)/(1+POWER(A12/_C,_B))</f>
-        <v>50.586727215774317</v>
+        <f>IF(ISBLANK(A12),0,_D+(_A-_D)/(1+POWER(A12/_C,_B)))</f>
+        <v>50.654525648316636</v>
       </c>
       <c r="D12">
         <f t="shared" si="0"/>
-        <v>1.5782516731794002E-3</v>
+        <v>3.792503734873414E-4</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>0.25581395348837199</v>
+        <v>0.23923444976076499</v>
       </c>
       <c r="B13">
-        <v>50.361999999999902</v>
+        <v>50.657999999999902</v>
       </c>
       <c r="C13">
-        <f>_D+(_A-_D)/(1+POWER(A13/_C,_B))</f>
-        <v>50.357576279510525</v>
+        <f>IF(ISBLANK(A13),0,_D+(_A-_D)/(1+POWER(A13/_C,_B)))</f>
+        <v>50.653682928113923</v>
       </c>
       <c r="D13">
         <f t="shared" si="0"/>
-        <v>1.9569302968138826E-5</v>
+        <v>1.8637109668705162E-5</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>0.38372093023255799</v>
+        <v>0.36363636363636298</v>
       </c>
       <c r="B14">
-        <v>49.961999999999897</v>
+        <v>50.622999999999898</v>
       </c>
       <c r="C14">
-        <f>_D+(_A-_D)/(1+POWER(A14/_C,_B))</f>
-        <v>49.917025894451392</v>
+        <f>IF(ISBLANK(A14),0,_D+(_A-_D)/(1+POWER(A14/_C,_B)))</f>
+        <v>50.639919803518204</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
-        <v>2.0226701698880588E-3</v>
+        <f t="shared" ref="D14:D24" si="1">POWER(C14-B14,2)</f>
+        <v>2.8627975109807329E-4</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>0.59302325581395299</v>
+        <v>0.42105263157894701</v>
       </c>
       <c r="B15">
-        <v>49.436</v>
+        <v>50.580999999999896</v>
       </c>
       <c r="C15">
-        <f>_D+(_A-_D)/(1+POWER(A15/_C,_B))</f>
-        <v>49.437775364875939</v>
+        <f>IF(ISBLANK(A15),0,_D+(_A-_D)/(1+POWER(A15/_C,_B)))</f>
+        <v>50.615476442121121</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
-        <v>3.1519204427198345E-6</v>
+        <f t="shared" si="1"/>
+        <v>1.1886250613381561E-3</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>0.70930232558139505</v>
+        <v>0.46411483253588498</v>
       </c>
       <c r="B16">
-        <v>49.317</v>
+        <v>50.538999999999902</v>
       </c>
       <c r="C16">
-        <f>_D+(_A-_D)/(1+POWER(A16/_C,_B))</f>
-        <v>49.315507514739672</v>
+        <f>IF(ISBLANK(A16),0,_D+(_A-_D)/(1+POWER(A16/_C,_B)))</f>
+        <v>50.580543129138263</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
-        <v>2.2275122522982346E-6</v>
+        <f t="shared" si="1"/>
+        <v>1.7258315786065574E-3</v>
       </c>
       <c r="H16" s="1"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>0.82558139534883701</v>
+        <v>0.52631578947368396</v>
       </c>
       <c r="B17">
-        <v>49.256</v>
+        <v>50.461999999999897</v>
       </c>
       <c r="C17">
-        <f>_D+(_A-_D)/(1+POWER(A17/_C,_B))</f>
-        <v>49.245698452572888</v>
+        <f>IF(ISBLANK(A17),0,_D+(_A-_D)/(1+POWER(A17/_C,_B)))</f>
+        <v>50.491574295022247</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
-        <v>1.0612187939303286E-4</v>
+        <f t="shared" si="1"/>
+        <v>8.7463892606898849E-4</v>
       </c>
       <c r="H17" s="1"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>0.94186046511627897</v>
+        <v>0.602870813397129</v>
       </c>
       <c r="B18">
-        <v>49.222999999999999</v>
+        <v>50.34</v>
       </c>
       <c r="C18">
-        <f>_D+(_A-_D)/(1+POWER(A18/_C,_B))</f>
-        <v>49.204392461448776</v>
+        <f>IF(ISBLANK(A18),0,_D+(_A-_D)/(1+POWER(A18/_C,_B)))</f>
+        <v>50.304616627082346</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
-        <v>3.4624049093523327E-4</v>
+        <f t="shared" si="1"/>
+        <v>1.2519830790299928E-3</v>
       </c>
       <c r="H18" s="1"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
+        <v>0.68899521531100405</v>
+      </c>
+      <c r="B19">
+        <v>50.09</v>
+      </c>
+      <c r="C19">
+        <f>IF(ISBLANK(A19),0,_D+(_A-_D)/(1+POWER(A19/_C,_B)))</f>
+        <v>50.019155844334179</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>5.0188943920035541E-3</v>
+      </c>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>0.72727272727272696</v>
+      </c>
+      <c r="B20">
+        <v>49.835000000000001</v>
+      </c>
+      <c r="C20">
+        <f>IF(ISBLANK(A20),0,_D+(_A-_D)/(1+POWER(A20/_C,_B)))</f>
+        <v>49.88978625402887</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>3.0015336305157705E-3</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>0.81339712918660201</v>
+      </c>
+      <c r="B21">
+        <v>49.633000000000003</v>
+      </c>
+      <c r="C21">
+        <f>IF(ISBLANK(A21),0,_D+(_A-_D)/(1+POWER(A21/_C,_B)))</f>
+        <v>49.643465936849829</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>1.0953583414454802E-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>0.88038277511961704</v>
+      </c>
+      <c r="B22">
+        <v>49.481999999999999</v>
+      </c>
+      <c r="C22">
+        <f>IF(ISBLANK(A22),0,_D+(_A-_D)/(1+POWER(A22/_C,_B)))</f>
+        <v>49.509229532306399</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>7.4144742962528229E-4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>0.93301435406698496</v>
+      </c>
+      <c r="B23">
+        <v>49.4269999999999</v>
+      </c>
+      <c r="C23">
+        <f>IF(ISBLANK(A23),0,_D+(_A-_D)/(1+POWER(A23/_C,_B)))</f>
+        <v>49.435294422396581</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>6.879744289455584E-5</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24">
         <v>1</v>
       </c>
-      <c r="B19">
-        <v>49.211999999999897</v>
-      </c>
-      <c r="C19">
-        <f>_D+(_A-_D)/(1+POWER(A19/_C,_B))</f>
-        <v>49.190178276201856</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="0"/>
-        <v>4.7618762951799539E-4</v>
-      </c>
-      <c r="H19" s="1"/>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2"/>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2"/>
+      <c r="B24">
+        <v>49.406999999999996</v>
+      </c>
+      <c r="C24">
+        <f>IF(ISBLANK(A24),0,_D+(_A-_D)/(1+POWER(A24/_C,_B)))</f>
+        <v>49.371073513231082</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>1.2907124515570143E-3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
work with normalised data
</commit_message>
<xml_diff>
--- a/data/cant_solve_txt_4PL.xlsx
+++ b/data/cant_solve_txt_4PL.xlsx
@@ -7,16 +7,16 @@
     <workbookView xWindow="360" yWindow="120" windowWidth="23955" windowHeight="13110"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Fitter" sheetId="1" r:id="rId1"/>
+    <sheet name="gradients" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_A">Sheet1!$D$3</definedName>
-    <definedName name="_B">Sheet1!$D$4</definedName>
-    <definedName name="_C">Sheet1!$D$5</definedName>
-    <definedName name="_D">Sheet1!$D$6</definedName>
-    <definedName name="solver_adj" localSheetId="0" hidden="1">Sheet1!$D$3:$D$6</definedName>
+    <definedName name="_A">Fitter!$D$3</definedName>
+    <definedName name="_B">Fitter!$D$4</definedName>
+    <definedName name="_C">Fitter!$D$5</definedName>
+    <definedName name="_D">Fitter!$D$6</definedName>
+    <definedName name="solver_adj" localSheetId="0" hidden="1">Fitter!$D$3:$D$6</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_eng" localSheetId="0" hidden="1">1</definedName>
@@ -30,7 +30,7 @@
     <definedName name="solver_nod" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
-    <definedName name="solver_opt" localSheetId="0" hidden="1">Sheet1!$D$7</definedName>
+    <definedName name="solver_opt" localSheetId="0" hidden="1">Fitter!$D$7</definedName>
     <definedName name="solver_pre" localSheetId="0" hidden="1">0.000001</definedName>
     <definedName name="solver_rbv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
@@ -49,7 +49,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>X</t>
   </si>
@@ -80,6 +80,24 @@
   <si>
     <t>base freq:</t>
   </si>
+  <si>
+    <t>tDelta</t>
+  </si>
+  <si>
+    <t>yDelta</t>
+  </si>
+  <si>
+    <t>td2</t>
+  </si>
+  <si>
+    <t>yd2</t>
+  </si>
+  <si>
+    <t>grad 1</t>
+  </si>
+  <si>
+    <t>grad 2</t>
+  </si>
 </sst>
 </file>
 
@@ -102,7 +120,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -110,14 +128,82 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,90 +251,78 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$21</c:f>
+              <c:f>(Fitter!$A$10:$A$21,Fitter!$L$29:$L$38)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9138755980861202E-2</c:v>
+                  <c:v>5.8139534883720902E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.105263157894736</c:v>
+                  <c:v>0.17441860465116199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23923444976076499</c:v>
+                  <c:v>0.290697674418604</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36363636363636298</c:v>
+                  <c:v>0.40697674418604601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42105263157894701</c:v>
+                  <c:v>0.61627906976744096</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46411483253588498</c:v>
+                  <c:v>0.74418604651162701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.52631578947368396</c:v>
+                  <c:v>0.837209302325581</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.602870813397129</c:v>
+                  <c:v>0.95348837209302295</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.68899521531100405</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.72727272727272696</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.81339712918660201</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$10:$B$21</c:f>
+              <c:f>(Fitter!$B$10:$B$21,Fitter!$M$29:$M$38)</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="12"/>
+                <c:ptCount val="22"/>
                 <c:pt idx="0">
-                  <c:v>50.685000000000002</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.681999999999903</c:v>
+                  <c:v>7.3726541555120201E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.673999999999999</c:v>
+                  <c:v>2.9490616621991001E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.657999999999902</c:v>
+                  <c:v>7.0375335120654706E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.622999999999898</c:v>
+                  <c:v>0.150134048257382</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.580999999999896</c:v>
+                  <c:v>0.50268096514744598</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.538999999999902</c:v>
+                  <c:v>0.77077747989275502</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50.461999999999897</c:v>
+                  <c:v>0.89477211796246003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50.34</c:v>
+                  <c:v>0.97922252010723398</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.09</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>49.835000000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>49.633000000000003</c:v>
+                  <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -268,53 +342,38 @@
           </c:spPr>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$A$10:$A$24</c:f>
+              <c:f>(Fitter!$A$10:$A$24,Fitter!$L$29:$L$38)</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="15"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.9138755980861202E-2</c:v>
+                  <c:v>5.8139534883720902E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.105263157894736</c:v>
+                  <c:v>0.17441860465116199</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.23923444976076499</c:v>
+                  <c:v>0.290697674418604</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.36363636363636298</c:v>
+                  <c:v>0.40697674418604601</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.42105263157894701</c:v>
+                  <c:v>0.61627906976744096</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.46411483253588498</c:v>
+                  <c:v>0.74418604651162701</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.52631578947368396</c:v>
+                  <c:v>0.837209302325581</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.602870813397129</c:v>
+                  <c:v>0.95348837209302295</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.68899521531100405</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>0.72727272727272696</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>0.81339712918660201</c:v>
-                </c:pt>
-                <c:pt idx="12" formatCode="General">
-                  <c:v>0.88038277511961704</c:v>
-                </c:pt>
-                <c:pt idx="13" formatCode="General">
-                  <c:v>0.93301435406698496</c:v>
-                </c:pt>
-                <c:pt idx="14" formatCode="General">
                   <c:v>1</c:v>
                 </c:pt>
               </c:numCache>
@@ -322,55 +381,83 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$C$10:$C$24</c:f>
+              <c:f>Fitter!$C$10:$C$24</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="15"/>
                 <c:pt idx="0">
-                  <c:v>50.654528760564574</c:v>
+                  <c:v>1.8020753348302776E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>50.654528760537161</c:v>
+                  <c:v>1.8044024827801319E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>50.654525648316636</c:v>
+                  <c:v>2.1210230113475559E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>50.653682928113923</c:v>
+                  <c:v>4.8723267217313904E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>50.639919803518204</c:v>
+                  <c:v>0.14463030810024735</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>50.615476442121121</c:v>
+                  <c:v>0.52419713714875626</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>50.580543129138263</c:v>
+                  <c:v>0.75754087649985147</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>50.491574295022247</c:v>
+                  <c:v>0.88026679770089244</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>50.304616627082346</c:v>
+                  <c:v>0.98188491437839365</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>50.019155844334179</c:v>
+                  <c:v>1.0102973676274047</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>49.88978625402887</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>49.643465936849829</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>49.509229532306399</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>49.435294422396581</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>49.371073513231082</c:v>
-                </c:pt>
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="28575">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Fitter!$L$29:$L$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Fitter!$M$29:$M$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="6"/>
               </c:numCache>
             </c:numRef>
           </c:yVal>
@@ -384,11 +471,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="297686912"/>
-        <c:axId val="297688448"/>
+        <c:axId val="304048000"/>
+        <c:axId val="304049536"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="297686912"/>
+        <c:axId val="304048000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -398,12 +485,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297688448"/>
+        <c:crossAx val="304049536"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="297688448"/>
+        <c:axId val="304049536"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -414,7 +501,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="297686912"/>
+        <c:crossAx val="304048000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -834,14 +921,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:H24"/>
+  <dimension ref="A3:M38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="C25" sqref="C25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="15.85546875" customWidth="1"/>
     <col min="6" max="6" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -850,7 +938,7 @@
         <v>2</v>
       </c>
       <c r="D3">
-        <v>50.654528760564574</v>
+        <v>1.8020753348302884E-2</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -858,7 +946,7 @@
         <v>3</v>
       </c>
       <c r="D4">
-        <v>6.8279031260186276</v>
+        <v>4.4812743699311435</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,7 +954,7 @@
         <v>4</v>
       </c>
       <c r="D5">
-        <v>0.70871416441597912</v>
+        <v>0.64629961950721071</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
@@ -874,7 +962,7 @@
         <v>5</v>
       </c>
       <c r="D6">
-        <v>49.248777592008274</v>
+        <v>1.1506223679482981</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
@@ -883,14 +971,14 @@
       </c>
       <c r="D7">
         <f>SUM(D10:D24)</f>
-        <v>1.7639332490389022E-2</v>
+        <v>1.9679754703749689E-3</v>
       </c>
       <c r="F7" t="s">
         <v>9</v>
       </c>
       <c r="G7">
         <f>_D+(_A-_D)/(1+POWER(_C/_C,_B))</f>
-        <v>49.951653176286428</v>
+        <v>0.58432156064830043</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
@@ -912,250 +1000,262 @@
         <v>0</v>
       </c>
       <c r="B10">
-        <v>50.685000000000002</v>
+        <v>0</v>
       </c>
       <c r="C10">
-        <f>IF(ISBLANK(A10),0,_D+(_A-_D)/(1+POWER(A10/_C,_B)))</f>
-        <v>50.654528760564574</v>
+        <f t="shared" ref="C10:C24" si="0">IF(ISBLANK(A10),0,_D+(_A-_D)/(1+POWER(A10/_C,_B)))</f>
+        <v>1.8020753348302776E-2</v>
       </c>
       <c r="D10">
         <f>POWER(C10-B10,2)</f>
-        <v>9.2849643273120006E-4</v>
+        <v>3.247475512403657E-4</v>
       </c>
       <c r="H10" s="1"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
-        <v>1.9138755980861202E-2</v>
+        <v>5.8139534883720902E-2</v>
       </c>
       <c r="B11">
-        <v>50.681999999999903</v>
+        <v>7.3726541555120201E-3</v>
       </c>
       <c r="C11">
-        <f>IF(ISBLANK(A11),0,_D+(_A-_D)/(1+POWER(A11/_C,_B)))</f>
-        <v>50.654528760537161</v>
+        <f t="shared" si="0"/>
+        <v>1.8044024827801319E-2</v>
       </c>
       <c r="D11">
-        <f t="shared" ref="D11:D19" si="0">POWER(C11-B11,2)</f>
-        <v>7.5466899761928244E-4</v>
+        <f t="shared" ref="D11:D13" si="1">POWER(C11-B11,2)</f>
+        <v>1.1387815202539619E-4</v>
       </c>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
-        <v>0.105263157894736</v>
+        <v>0.17441860465116199</v>
       </c>
       <c r="B12">
-        <v>50.673999999999999</v>
+        <v>2.9490616621991001E-2</v>
       </c>
       <c r="C12">
-        <f>IF(ISBLANK(A12),0,_D+(_A-_D)/(1+POWER(A12/_C,_B)))</f>
-        <v>50.654525648316636</v>
+        <f t="shared" si="0"/>
+        <v>2.1210230113475559E-2</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
-        <v>3.792503734873414E-4</v>
+        <f t="shared" si="1"/>
+        <v>6.8564800730404552E-5</v>
       </c>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
-        <v>0.23923444976076499</v>
+        <v>0.290697674418604</v>
       </c>
       <c r="B13">
-        <v>50.657999999999902</v>
+        <v>7.0375335120654706E-2</v>
       </c>
       <c r="C13">
-        <f>IF(ISBLANK(A13),0,_D+(_A-_D)/(1+POWER(A13/_C,_B)))</f>
-        <v>50.653682928113923</v>
+        <f t="shared" si="0"/>
+        <v>4.8723267217313904E-2</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
-        <v>1.8637109668705162E-5</v>
+        <f t="shared" si="1"/>
+        <v>4.6881204449088096E-4</v>
       </c>
       <c r="H13" s="1"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
-        <v>0.36363636363636298</v>
+        <v>0.40697674418604601</v>
       </c>
       <c r="B14">
-        <v>50.622999999999898</v>
+        <v>0.150134048257382</v>
       </c>
       <c r="C14">
-        <f>IF(ISBLANK(A14),0,_D+(_A-_D)/(1+POWER(A14/_C,_B)))</f>
-        <v>50.639919803518204</v>
+        <f t="shared" si="0"/>
+        <v>0.14463030810024735</v>
       </c>
       <c r="D14">
-        <f t="shared" ref="D14:D24" si="1">POWER(C14-B14,2)</f>
-        <v>2.8627975109807329E-4</v>
+        <f t="shared" ref="D14:D24" si="2">POWER(C14-B14,2)</f>
+        <v>3.0291155717256494E-5</v>
       </c>
       <c r="H14" s="1"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
-        <v>0.42105263157894701</v>
+        <v>0.61627906976744096</v>
       </c>
       <c r="B15">
-        <v>50.580999999999896</v>
+        <v>0.50268096514744598</v>
       </c>
       <c r="C15">
-        <f>IF(ISBLANK(A15),0,_D+(_A-_D)/(1+POWER(A15/_C,_B)))</f>
-        <v>50.615476442121121</v>
+        <f t="shared" si="0"/>
+        <v>0.52419713714875626</v>
       </c>
       <c r="D15">
-        <f t="shared" si="1"/>
-        <v>1.1886250613381561E-3</v>
+        <f t="shared" si="2"/>
+        <v>4.6294565758996862E-4</v>
       </c>
       <c r="H15" s="1"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
-        <v>0.46411483253588498</v>
+        <v>0.74418604651162701</v>
       </c>
       <c r="B16">
-        <v>50.538999999999902</v>
+        <v>0.77077747989275502</v>
       </c>
       <c r="C16">
-        <f>IF(ISBLANK(A16),0,_D+(_A-_D)/(1+POWER(A16/_C,_B)))</f>
-        <v>50.580543129138263</v>
+        <f t="shared" si="0"/>
+        <v>0.75754087649985147</v>
       </c>
       <c r="D16">
-        <f t="shared" si="1"/>
-        <v>1.7258315786065574E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.7520766938102596E-4</v>
       </c>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
-        <v>0.52631578947368396</v>
+        <v>0.837209302325581</v>
       </c>
       <c r="B17">
-        <v>50.461999999999897</v>
+        <v>0.89477211796246003</v>
       </c>
       <c r="C17">
-        <f>IF(ISBLANK(A17),0,_D+(_A-_D)/(1+POWER(A17/_C,_B)))</f>
-        <v>50.491574295022247</v>
+        <f t="shared" si="0"/>
+        <v>0.88026679770089244</v>
       </c>
       <c r="D17">
-        <f t="shared" si="1"/>
-        <v>8.7463892606898849E-4</v>
+        <f t="shared" si="2"/>
+        <v>2.1040431589064323E-4</v>
       </c>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
-        <v>0.602870813397129</v>
+        <v>0.95348837209302295</v>
       </c>
       <c r="B18">
-        <v>50.34</v>
+        <v>0.97922252010723398</v>
       </c>
       <c r="C18">
-        <f>IF(ISBLANK(A18),0,_D+(_A-_D)/(1+POWER(A18/_C,_B)))</f>
-        <v>50.304616627082346</v>
+        <f t="shared" si="0"/>
+        <v>0.98188491437839365</v>
       </c>
       <c r="D18">
-        <f t="shared" si="1"/>
-        <v>1.2519830790299928E-3</v>
+        <f t="shared" si="2"/>
+        <v>7.0883432551037915E-6</v>
       </c>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
-        <v>0.68899521531100405</v>
+        <v>1</v>
       </c>
       <c r="B19">
-        <v>50.09</v>
+        <v>1</v>
       </c>
       <c r="C19">
-        <f>IF(ISBLANK(A19),0,_D+(_A-_D)/(1+POWER(A19/_C,_B)))</f>
-        <v>50.019155844334179</v>
+        <f t="shared" si="0"/>
+        <v>1.0102973676274047</v>
       </c>
       <c r="D19">
-        <f t="shared" si="1"/>
-        <v>5.0188943920035541E-3</v>
+        <f t="shared" si="2"/>
+        <v>1.0603578005392314E-4</v>
       </c>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>0.72727272727272696</v>
-      </c>
-      <c r="B20">
-        <v>49.835000000000001</v>
-      </c>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
       <c r="C20">
-        <f>IF(ISBLANK(A20),0,_D+(_A-_D)/(1+POWER(A20/_C,_B)))</f>
-        <v>49.88978625402887</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D20">
-        <f t="shared" si="1"/>
-        <v>3.0015336305157705E-3</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>0.81339712918660201</v>
-      </c>
-      <c r="B21">
-        <v>49.633000000000003</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
       <c r="C21">
-        <f>IF(ISBLANK(A21),0,_D+(_A-_D)/(1+POWER(A21/_C,_B)))</f>
-        <v>49.643465936849829</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D21">
-        <f t="shared" si="1"/>
-        <v>1.0953583414454802E-4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22">
-        <v>0.88038277511961704</v>
-      </c>
-      <c r="B22">
-        <v>49.481999999999999</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C22">
-        <f>IF(ISBLANK(A22),0,_D+(_A-_D)/(1+POWER(A22/_C,_B)))</f>
-        <v>49.509229532306399</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D22">
-        <f t="shared" si="1"/>
-        <v>7.4144742962528229E-4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23">
-        <v>0.93301435406698496</v>
-      </c>
-      <c r="B23">
-        <v>49.4269999999999</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C23">
-        <f>IF(ISBLANK(A23),0,_D+(_A-_D)/(1+POWER(A23/_C,_B)))</f>
-        <v>49.435294422396581</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D23">
-        <f t="shared" si="1"/>
-        <v>6.879744289455584E-5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24">
-        <v>1</v>
-      </c>
-      <c r="B24">
-        <v>49.406999999999996</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="C24">
-        <f>IF(ISBLANK(A24),0,_D+(_A-_D)/(1+POWER(A24/_C,_B)))</f>
-        <v>49.371073513231082</v>
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="D24">
-        <f t="shared" si="1"/>
-        <v>1.2907124515570143E-3</v>
-      </c>
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L29" s="3"/>
+      <c r="M29" s="4"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L30" s="5"/>
+      <c r="M30" s="6"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L31" s="5"/>
+      <c r="M31" s="6"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="L32" s="5"/>
+      <c r="M32" s="6"/>
+    </row>
+    <row r="33" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L33" s="5"/>
+      <c r="M33" s="6"/>
+    </row>
+    <row r="34" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L34" s="5"/>
+      <c r="M34" s="6"/>
+    </row>
+    <row r="35" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L35" s="5"/>
+      <c r="M35" s="6"/>
+    </row>
+    <row r="36" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L36" s="5"/>
+      <c r="M36" s="6"/>
+    </row>
+    <row r="37" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L37" s="5"/>
+      <c r="M37" s="6"/>
+    </row>
+    <row r="38" spans="12:13" x14ac:dyDescent="0.25">
+      <c r="L38" s="7"/>
+      <c r="M38" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1165,12 +1265,355 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:H11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>5.8139534883720902E-2</v>
+      </c>
+      <c r="B3">
+        <v>7.3726541555120201E-3</v>
+      </c>
+      <c r="C3" s="2">
+        <f>A3-A2</f>
+        <v>5.8139534883720902E-2</v>
+      </c>
+      <c r="D3">
+        <f>B3-B2</f>
+        <v>7.3726541555120201E-3</v>
+      </c>
+      <c r="E3">
+        <f>D3/C3</f>
+        <v>0.1268096514748068</v>
+      </c>
+      <c r="F3" s="2">
+        <f>C3</f>
+        <v>5.8139534883720902E-2</v>
+      </c>
+      <c r="G3">
+        <f>D3-D2</f>
+        <v>7.3726541555120201E-3</v>
+      </c>
+      <c r="H3">
+        <f>G3/F3</f>
+        <v>0.1268096514748068</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>0.17441860465116199</v>
+      </c>
+      <c r="B4">
+        <v>2.9490616621991001E-2</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C11" si="0">A4-A3</f>
+        <v>0.1162790697674411</v>
+      </c>
+      <c r="D4">
+        <f t="shared" ref="D4:D11" si="1">B4-B3</f>
+        <v>2.2117962466478982E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" ref="E4:E11" si="2">D4/C4</f>
+        <v>0.1902144772117205</v>
+      </c>
+      <c r="F4" s="2">
+        <f t="shared" ref="F4:F11" si="3">C4</f>
+        <v>0.1162790697674411</v>
+      </c>
+      <c r="G4">
+        <f t="shared" ref="G4:G11" si="4">D4-D3</f>
+        <v>1.4745308310966963E-2</v>
+      </c>
+      <c r="H4">
+        <f t="shared" ref="H4:H11" si="5">G4/F4</f>
+        <v>0.12680965147431672</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>0.290697674418604</v>
+      </c>
+      <c r="B5">
+        <v>7.0375335120654706E-2</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11627906976744201</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>4.0884718498663708E-2</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="2"/>
+        <v>0.35160857908850746</v>
+      </c>
+      <c r="F5" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11627906976744201</v>
+      </c>
+      <c r="G5">
+        <f t="shared" si="4"/>
+        <v>1.8766756032184726E-2</v>
+      </c>
+      <c r="H5">
+        <f t="shared" si="5"/>
+        <v>0.16139410187678843</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>0.40697674418604601</v>
+      </c>
+      <c r="B6">
+        <v>0.150134048257382</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11627906976744201</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="1"/>
+        <v>7.9758713136727291E-2</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="2"/>
+        <v>0.68592493297585377</v>
+      </c>
+      <c r="F6" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11627906976744201</v>
+      </c>
+      <c r="G6">
+        <f t="shared" si="4"/>
+        <v>3.8873994638063583E-2</v>
+      </c>
+      <c r="H6">
+        <f t="shared" si="5"/>
+        <v>0.33431635388734637</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>0.61627906976744096</v>
+      </c>
+      <c r="B7">
+        <v>0.50268096514744598</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.20930232558139494</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="1"/>
+        <v>0.35254691689006401</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="2"/>
+        <v>1.6843908251414201</v>
+      </c>
+      <c r="F7" s="2">
+        <f t="shared" si="3"/>
+        <v>0.20930232558139494</v>
+      </c>
+      <c r="G7">
+        <f t="shared" si="4"/>
+        <v>0.27278820375333673</v>
+      </c>
+      <c r="H7">
+        <f t="shared" si="5"/>
+        <v>1.3033214179326114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>0.74418604651162701</v>
+      </c>
+      <c r="B8">
+        <v>0.77077747989275502</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.12790697674418605</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="1"/>
+        <v>0.26809651474530904</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="2"/>
+        <v>2.0960272970996887</v>
+      </c>
+      <c r="F8" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12790697674418605</v>
+      </c>
+      <c r="G8">
+        <f t="shared" si="4"/>
+        <v>-8.4450402144754966E-2</v>
+      </c>
+      <c r="H8">
+        <f t="shared" si="5"/>
+        <v>-0.66024859858626606</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>0.837209302325581</v>
+      </c>
+      <c r="B9">
+        <v>0.89477211796246003</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="0"/>
+        <v>9.3023255813953987E-2</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="1"/>
+        <v>0.12399463806970501</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="2"/>
+        <v>1.3329423592493217</v>
+      </c>
+      <c r="F9" s="2">
+        <f t="shared" si="3"/>
+        <v>9.3023255813953987E-2</v>
+      </c>
+      <c r="G9">
+        <f t="shared" si="4"/>
+        <v>-0.14410187667560403</v>
+      </c>
+      <c r="H9">
+        <f t="shared" si="5"/>
+        <v>-1.549095174262735</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>0.95348837209302295</v>
+      </c>
+      <c r="B10">
+        <v>0.97922252010723398</v>
+      </c>
+      <c r="C10" s="2">
+        <f t="shared" si="0"/>
+        <v>0.11627906976744196</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>8.4450402144773951E-2</v>
+      </c>
+      <c r="E10">
+        <f t="shared" si="2"/>
+        <v>0.72627345844505542</v>
+      </c>
+      <c r="F10" s="2">
+        <f t="shared" si="3"/>
+        <v>0.11627906976744196</v>
+      </c>
+      <c r="G10">
+        <f t="shared" si="4"/>
+        <v>-3.9544235924931059E-2</v>
+      </c>
+      <c r="H10">
+        <f t="shared" si="5"/>
+        <v>-0.34008042895440682</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11" s="2">
+        <f t="shared" si="0"/>
+        <v>4.6511627906977049E-2</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2.0777479892766015E-2</v>
+      </c>
+      <c r="E11">
+        <f t="shared" si="2"/>
+        <v>0.44671581769446639</v>
+      </c>
+      <c r="F11" s="2">
+        <f t="shared" si="3"/>
+        <v>4.6511627906977049E-2</v>
+      </c>
+      <c r="G11">
+        <f t="shared" si="4"/>
+        <v>-6.3672922252007935E-2</v>
+      </c>
+      <c r="H11">
+        <f t="shared" si="5"/>
+        <v>-1.3689678284181617</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>